<commit_message>
added diffusion constants and sources
</commit_message>
<xml_diff>
--- a/ErkParams.xlsx
+++ b/ErkParams.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="979" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kdiff" sheetId="1" state="visible" r:id="rId2"/>
@@ -1599,7 +1599,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1686,6 +1686,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF5B9BD5"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1737,7 +1743,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF66"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -1784,8 +1790,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFEEEEEE"/>
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFD4DBDE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1930,11 +1936,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1950,7 +1952,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1958,11 +1964,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1970,7 +1976,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1982,12 +1988,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1995,6 +1997,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2010,7 +2016,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -2023,11 +2029,11 @@
       <rgbColor rgb="FF548235"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF5B9BD5"/>
       <rgbColor rgb="FFFF3333"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFCCFF66"/>
       <rgbColor rgb="FFDAE3F3"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -2035,7 +2041,7 @@
       <rgbColor rgb="FFD4DBDE"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFCCFF66"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -2077,7 +2083,7 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -2545,10 +2551,10 @@
   </sheetPr>
   <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1530" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1530" topLeftCell="A7" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3224,32 +3230,29 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" s="26" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="20" t="n">
+      <c r="C29" s="25" t="n">
         <v>0.06</v>
       </c>
-      <c r="D29" s="25" t="n">
+      <c r="D29" s="24" t="n">
         <v>0.5</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="20" t="n">
+      <c r="G29" s="25" t="n">
         <v>200</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25" t="s">
+      <c r="I29" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="K29" s="26" t="s">
+      <c r="K29" s="24" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3288,7 +3291,7 @@
       <c r="K30" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="L30" s="27" t="n">
+      <c r="L30" s="26" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -3303,7 +3306,7 @@
         <f aca="false">(D31+E31)/F31</f>
         <v>0.009375</v>
       </c>
-      <c r="D31" s="28" t="n">
+      <c r="D31" s="27" t="n">
         <f aca="false">4*E31</f>
         <v>1.2</v>
       </c>
@@ -3313,7 +3316,7 @@
       <c r="F31" s="0" t="n">
         <v>160</v>
       </c>
-      <c r="G31" s="29" t="n">
+      <c r="G31" s="28" t="n">
         <v>180</v>
       </c>
       <c r="H31" s="11" t="n">
@@ -3325,7 +3328,7 @@
       <c r="J31" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="L31" s="27" t="n">
+      <c r="L31" s="26" t="n">
         <v>1000001</v>
       </c>
     </row>
@@ -3340,7 +3343,7 @@
         <f aca="false">(D32+E32)/F32</f>
         <v>0.009375</v>
       </c>
-      <c r="D32" s="28" t="n">
+      <c r="D32" s="27" t="n">
         <f aca="false">4*E32</f>
         <v>1.2</v>
       </c>
@@ -3358,289 +3361,289 @@
       <c r="J32" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="L32" s="27" t="n">
+      <c r="L32" s="26" t="n">
         <v>1000002</v>
       </c>
     </row>
-    <row r="33" s="26" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="s">
+    <row r="33" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="20" t="n">
+      <c r="C33" s="31" t="n">
         <f aca="false">(D33+E33)/F33</f>
         <v>0.00625</v>
       </c>
-      <c r="D33" s="25" t="n">
+      <c r="D33" s="30" t="n">
         <f aca="false">4*E33</f>
         <v>0.8</v>
       </c>
-      <c r="E33" s="25" t="n">
+      <c r="E33" s="30" t="n">
         <v>0.2</v>
       </c>
-      <c r="F33" s="30" t="n">
+      <c r="F33" s="32" t="n">
         <v>160</v>
       </c>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25" t="s">
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="J33" s="32" t="s">
         <v>118</v>
       </c>
       <c r="L33" s="31" t="n">
         <v>1000003</v>
       </c>
     </row>
-    <row r="34" s="26" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24" t="s">
+    <row r="34" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="C34" s="20" t="n">
+      <c r="C34" s="31" t="n">
         <f aca="false">(D34+E34)/F34</f>
         <v>0.00625</v>
       </c>
-      <c r="D34" s="25" t="n">
+      <c r="D34" s="30" t="n">
         <f aca="false">4*E34</f>
         <v>0.8</v>
       </c>
-      <c r="E34" s="25" t="n">
+      <c r="E34" s="30" t="n">
         <v>0.2</v>
       </c>
-      <c r="F34" s="30" t="n">
+      <c r="F34" s="32" t="n">
         <v>160</v>
       </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25" t="s">
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="J34" s="32" t="s">
         <v>118</v>
       </c>
       <c r="L34" s="31" t="n">
         <v>1000004</v>
       </c>
     </row>
-    <row r="35" s="26" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24" t="s">
+    <row r="35" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="C35" s="20" t="n">
+      <c r="C35" s="31" t="n">
         <f aca="false">(D35+E35)/F35</f>
         <v>0.00191607587660471</v>
       </c>
-      <c r="D35" s="25" t="n">
+      <c r="D35" s="30" t="n">
         <f aca="false">4*E35</f>
         <v>24</v>
       </c>
-      <c r="E35" s="25" t="n">
+      <c r="E35" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="F35" s="20" t="n">
+      <c r="F35" s="31" t="n">
         <v>15657</v>
       </c>
-      <c r="G35" s="20" t="n">
+      <c r="G35" s="31" t="n">
         <v>150.00075</v>
       </c>
-      <c r="H35" s="25" t="s">
+      <c r="H35" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="I35" s="25" t="s">
+      <c r="I35" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J35" s="26" t="s">
+      <c r="J35" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="K35" s="26" t="s">
+      <c r="K35" s="32" t="s">
         <v>155</v>
       </c>
       <c r="L35" s="31" t="n">
         <v>1000005</v>
       </c>
     </row>
-    <row r="36" s="26" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="24" t="s">
+    <row r="36" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="20" t="n">
+      <c r="C36" s="31" t="n">
         <f aca="false">(D36+E36)/F36</f>
         <v>0.00191082802547771</v>
       </c>
-      <c r="D36" s="25" t="n">
+      <c r="D36" s="30" t="n">
         <f aca="false">4*E36</f>
         <v>24</v>
       </c>
-      <c r="E36" s="25" t="n">
+      <c r="E36" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="F36" s="20" t="n">
+      <c r="F36" s="31" t="n">
         <v>15700</v>
       </c>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25" t="s">
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J36" s="26" t="s">
+      <c r="J36" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="K36" s="26" t="s">
+      <c r="K36" s="30" t="s">
         <v>158</v>
       </c>
       <c r="L36" s="31" t="n">
         <v>1000006</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="32" t="s">
+    <row r="37" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C37" s="17" t="n">
+      <c r="C37" s="31" t="n">
         <f aca="false">(D37+E37)/F37</f>
         <v>0.0323974082073434</v>
       </c>
-      <c r="D37" s="28" t="n">
+      <c r="D37" s="30" t="n">
         <f aca="false">4*E37</f>
         <v>1.2</v>
       </c>
-      <c r="E37" s="11" t="n">
+      <c r="E37" s="30" t="n">
         <v>0.3</v>
       </c>
-      <c r="F37" s="27" t="n">
+      <c r="F37" s="31" t="n">
         <v>46.3</v>
       </c>
-      <c r="G37" s="20" t="n">
+      <c r="G37" s="31" t="n">
         <v>360.00252</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="I37" s="11" t="s">
+      <c r="I37" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J37" s="0" t="s">
+      <c r="J37" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="L37" s="27" t="n">
+      <c r="L37" s="31" t="n">
         <v>1000007</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="32" t="s">
+    <row r="38" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="C38" s="17" t="n">
+      <c r="C38" s="31" t="n">
         <f aca="false">(D38+E38)/F38</f>
         <v>0.0323974082073434</v>
       </c>
-      <c r="D38" s="28" t="n">
+      <c r="D38" s="30" t="n">
         <f aca="false">4*E38</f>
         <v>1.2</v>
       </c>
-      <c r="E38" s="11" t="n">
+      <c r="E38" s="30" t="n">
         <v>0.3</v>
       </c>
-      <c r="F38" s="27" t="n">
+      <c r="F38" s="31" t="n">
         <v>46.3</v>
       </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11" t="s">
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J38" s="0" t="s">
+      <c r="J38" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="L38" s="27" t="n">
+      <c r="L38" s="31" t="n">
         <v>1000008</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="33" t="s">
+    <row r="39" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="C39" s="17" t="n">
+      <c r="C39" s="31" t="n">
         <f aca="false">(D39+E39)/F39</f>
         <v>0.150375939849624</v>
       </c>
-      <c r="D39" s="28" t="n">
+      <c r="D39" s="30" t="n">
         <f aca="false">4*E39</f>
         <v>16</v>
       </c>
-      <c r="E39" s="11" t="n">
+      <c r="E39" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="F39" s="27" t="n">
+      <c r="F39" s="31" t="n">
         <v>133</v>
       </c>
-      <c r="G39" s="20" t="n">
+      <c r="G39" s="31" t="n">
         <v>15.000135</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H39" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="I39" s="11" t="s">
+      <c r="I39" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J39" s="0" t="s">
+      <c r="J39" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="L39" s="27" t="n">
+      <c r="L39" s="31" t="n">
         <v>1000009</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="33" t="s">
+    <row r="40" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="C40" s="17" t="n">
+      <c r="C40" s="31" t="n">
         <f aca="false">(D40+E40)/F40</f>
         <v>0.150375939849624</v>
       </c>
-      <c r="D40" s="28" t="n">
+      <c r="D40" s="30" t="n">
         <f aca="false">4*E40</f>
         <v>16</v>
       </c>
-      <c r="E40" s="11" t="n">
+      <c r="E40" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="F40" s="27" t="n">
+      <c r="F40" s="31" t="n">
         <v>133</v>
       </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11" t="s">
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="J40" s="0" t="s">
+      <c r="J40" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="L40" s="27" t="n">
+      <c r="L40" s="31" t="n">
         <v>1000010</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates were made- new reactions added, morphology file updated, Model file morphology parameters changed, ErkParams updated
</commit_message>
<xml_diff>
--- a/ErkParams.xlsx
+++ b/ErkParams.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="263">
   <si>
     <t xml:space="preserve">species id</t>
   </si>
@@ -1231,43 +1231,58 @@
     <t xml:space="preserve">Km=1 uM=1000 nM Vmax=10/sec;  This catalytic rate assumes that pDok is bound</t>
   </si>
   <si>
+    <t xml:space="preserve">Inactivation of Rap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RapGTP +SynGAP&lt;-&gt; RapGTP.Gap --&gt; SynGap+Rap(GDP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J Biol Chem. 2015 Feb 20;290(8):4908-27.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interpreted from figures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RasGTP +pSynGAP&lt;-&gt; RasGTP.Gap --&gt; pSynGap+Ras(GDP)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Walkup WG 4th, Washburn L, Sweredoski MJ, Carlisle HJ, Graham RL, Hess S, </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Kennedy MB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RapGTP +pSynGAP&lt;-&gt; RapGTP.Gap --&gt; pSynGap+Rap(GDP)</t>
+  </si>
+  <si>
     <t xml:space="preserve">CaMKII inhib SynGap</t>
   </si>
   <si>
     <t xml:space="preserve">CKpCamCa4+SynGap &lt;-&gt; CKpCamCa4+pSynGap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J Biol Chem. 2015 Feb 20;290(8):4908-27.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Walkup WG 4th, Washburn L, Sweredoski MJ, Carlisle HJ, Graham RL, Hess S, </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Kennedy MB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Calmodulin working through Pyk2</t>
@@ -1603,7 +1618,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1681,7 +1696,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFFC000"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1696,13 +1711,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1812,12 +1820,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -1846,7 +1861,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1871,148 +1886,160 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2069,7 +2096,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFC000"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFED7D31"/>
       <rgbColor rgb="FF666699"/>
@@ -2100,11 +2127,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="161.989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="158.479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,1261 +2587,1388 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1530" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1530" topLeftCell="A37" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+    <row r="2" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="10" t="n">
         <v>0.0002</v>
       </c>
-      <c r="D2" s="8" t="n">
+      <c r="D2" s="10" t="n">
         <v>0.1</v>
       </c>
-      <c r="G2" s="8" t="n">
+      <c r="G2" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+    <row r="3" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="10" t="n">
         <v>0.08</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="D3" s="10" t="n">
         <v>1.28</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="10" t="n">
         <v>0.32</v>
       </c>
-      <c r="G3" s="8" t="n">
+      <c r="G3" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+    <row r="4" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="10" t="n">
         <v>1.28</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C5" s="10" t="n">
         <v>0.48</v>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="D5" s="10" t="n">
         <v>7.68</v>
       </c>
-      <c r="E5" s="8" t="n">
+      <c r="E5" s="10" t="n">
         <v>1.92</v>
       </c>
-      <c r="G5" s="8" t="n">
+      <c r="G5" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="12" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="15" t="n">
+      <c r="C8" s="17" t="n">
         <v>0.000234</v>
       </c>
-      <c r="D8" s="13" t="n">
+      <c r="D8" s="15" t="n">
         <v>0.28</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="n">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13" t="s">
+      <c r="H8" s="15"/>
+      <c r="I8" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
+    <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="13" t="n">
+      <c r="C9" s="15" t="n">
         <v>0.012</v>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="15" t="n">
         <v>0.96</v>
       </c>
-      <c r="E9" s="13" t="n">
+      <c r="E9" s="15" t="n">
         <v>0.024</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="n">
+      <c r="F9" s="15"/>
+      <c r="G9" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13" t="s">
+      <c r="H9" s="15"/>
+      <c r="I9" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+    <row r="10" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="13" t="n">
+      <c r="C10" s="15" t="n">
         <f aca="false">0.04</f>
         <v>0.04</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="15" t="n">
         <v>8</v>
       </c>
-      <c r="E10" s="13" t="n">
+      <c r="E10" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="13" t="n">
+      <c r="F10" s="15" t="n">
         <f aca="false">(Sheet1!D10+Sheet1!E10)/Sheet1!C10</f>
         <v>250</v>
       </c>
-      <c r="G10" s="13" t="n">
+      <c r="G10" s="15" t="n">
         <v>12</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+    <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="19" t="n">
+      <c r="C13" s="21" t="n">
         <f aca="false">(Sheet1!D13+Sheet1!E13)/Sheet1!F13</f>
         <v>2.00400801603206</v>
       </c>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="15" t="n">
         <v>80</v>
       </c>
-      <c r="E13" s="13" t="n">
+      <c r="E13" s="15" t="n">
         <v>20</v>
       </c>
-      <c r="F13" s="19" t="n">
+      <c r="F13" s="21" t="n">
         <v>49.9</v>
       </c>
-      <c r="G13" s="19" t="n">
+      <c r="G13" s="21" t="n">
         <v>20</v>
       </c>
-      <c r="H13" s="13" t="n">
+      <c r="H13" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="13" t="n">
+      <c r="C14" s="15" t="n">
         <v>100</v>
       </c>
-      <c r="D14" s="13" t="n">
+      <c r="D14" s="15" t="n">
         <v>0.1</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="13" t="n">
+      <c r="C15" s="15" t="n">
         <f aca="false">(Sheet1!D15+Sheet1!E15)/Sheet1!F15</f>
         <v>0.0801998396003208</v>
       </c>
-      <c r="D15" s="13" t="n">
+      <c r="D15" s="15" t="n">
         <v>0.1</v>
       </c>
-      <c r="E15" s="13" t="n">
+      <c r="E15" s="15" t="n">
         <v>40</v>
       </c>
-      <c r="F15" s="13" t="n">
+      <c r="F15" s="15" t="n">
         <v>500.001</v>
       </c>
-      <c r="G15" s="19" t="n">
+      <c r="G15" s="21" t="n">
         <v>500</v>
       </c>
-      <c r="H15" s="13" t="n">
+      <c r="H15" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="13" t="n">
+      <c r="C16" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="D16" s="13" t="n">
+      <c r="D16" s="15" t="n">
         <v>0.01</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="13" t="n">
+      <c r="C17" s="15" t="n">
         <v>0.001</v>
       </c>
-      <c r="D17" s="13" t="n">
+      <c r="D17" s="15" t="n">
         <v>0.002</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13" t="s">
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H17" s="13" t="n">
+      <c r="H17" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="13" t="n">
+      <c r="C18" s="15" t="n">
         <v>0.001</v>
       </c>
-      <c r="D18" s="13" t="n">
+      <c r="D18" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13" t="n">
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15" t="n">
         <v>500</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13" t="s">
+      <c r="H18" s="15"/>
+      <c r="I18" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="19" t="n">
+      <c r="C19" s="21" t="n">
         <f aca="false">(Sheet1!D19+Sheet1!E19)/Sheet1!F19</f>
         <v>0.0400005600126402</v>
       </c>
-      <c r="D19" s="13" t="n">
+      <c r="D19" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="E19" s="13" t="n">
+      <c r="E19" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="F19" s="19" t="n">
+      <c r="F19" s="21" t="n">
         <v>9.9998599988</v>
       </c>
-      <c r="G19" s="19" t="n">
+      <c r="G19" s="21" t="n">
         <v>200</v>
       </c>
-      <c r="H19" s="13" t="n">
+      <c r="H19" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="13" t="n">
+      <c r="C20" s="15" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D20" s="13" t="n">
+      <c r="D20" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13" t="s">
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="15" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="21" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="19" t="n">
+      <c r="C21" s="21" t="n">
         <f aca="false">(Sheet1!D21+Sheet1!E21)/Sheet1!F21</f>
         <v>0.202000404016968</v>
       </c>
-      <c r="D21" s="13" t="n">
+      <c r="D21" s="15" t="n">
         <v>200</v>
       </c>
-      <c r="E21" s="13" t="n">
+      <c r="E21" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="F21" s="19" t="n">
+      <c r="F21" s="21" t="n">
         <v>999.99799992</v>
       </c>
-      <c r="G21" s="19" t="n">
+      <c r="G21" s="21" t="n">
         <v>12</v>
       </c>
-      <c r="H21" s="13" t="n">
+      <c r="H21" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="15" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="21" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="23" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="24" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="8" t="s">
+    <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="K26" s="0" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="K26" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="23" t="n">
+      <c r="C27" s="25" t="n">
         <v>0.06</v>
       </c>
-      <c r="D27" s="12" t="n">
+      <c r="D27" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="23" t="n">
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="25" t="n">
         <v>200</v>
       </c>
-      <c r="H27" s="12" t="n">
+      <c r="H27" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="I27" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="J27" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="24" t="s">
+    <row r="28" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="25" t="n">
+      <c r="C28" s="26" t="n">
         <v>0.06</v>
       </c>
-      <c r="D28" s="24" t="n">
+      <c r="D28" s="20" t="n">
         <v>0.5</v>
       </c>
-      <c r="G28" s="25" t="n">
+      <c r="G28" s="26" t="n">
         <v>200</v>
       </c>
-      <c r="I28" s="24" t="s">
+      <c r="I28" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="J28" s="24" t="s">
+      <c r="J28" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="K28" s="24" t="s">
+      <c r="K28" s="20" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="s">
+    <row r="29" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="27" t="n">
+      <c r="C29" s="28" t="n">
         <f aca="false">(Sheet1!D29+Sheet1!E29)/Sheet1!F29</f>
         <v>0.202202202202202</v>
       </c>
-      <c r="D29" s="26" t="n">
+      <c r="D29" s="27" t="n">
         <v>200</v>
       </c>
-      <c r="E29" s="12" t="n">
+      <c r="E29" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="7" t="n">
         <v>999</v>
       </c>
-      <c r="G29" s="23" t="n">
+      <c r="G29" s="25" t="n">
         <v>12</v>
       </c>
-      <c r="H29" s="12" t="n">
+      <c r="H29" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="K29" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="L29" s="28" t="n">
+      <c r="L29" s="29" t="n">
         <v>1000000</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="27" t="n">
+      <c r="C30" s="28" t="n">
         <f aca="false">(Sheet1!D30+Sheet1!E30)/Sheet1!F30</f>
         <v>0.009375</v>
       </c>
-      <c r="D30" s="30" t="n">
+      <c r="D30" s="31" t="n">
         <f aca="false">4*Sheet1!E30</f>
         <v>1.2</v>
       </c>
-      <c r="E30" s="12" t="n">
+      <c r="E30" s="14" t="n">
         <v>0.3</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="7" t="n">
         <v>160</v>
       </c>
-      <c r="G30" s="31" t="n">
+      <c r="G30" s="32" t="n">
         <v>180</v>
       </c>
-      <c r="H30" s="12" t="n">
+      <c r="H30" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="I30" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="J30" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="L30" s="28" t="n">
+      <c r="L30" s="29" t="n">
         <v>1000001</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C31" s="27" t="n">
+      <c r="C31" s="28" t="n">
         <f aca="false">(Sheet1!D31+Sheet1!E31)/Sheet1!F31</f>
         <v>0.009375</v>
       </c>
-      <c r="D31" s="30" t="n">
+      <c r="D31" s="31" t="n">
         <f aca="false">4*Sheet1!E31</f>
         <v>1.2</v>
       </c>
-      <c r="E31" s="12" t="n">
+      <c r="E31" s="14" t="n">
         <v>0.3</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="7" t="n">
         <v>160</v>
       </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12" t="s">
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="L31" s="28" t="n">
+      <c r="L31" s="29" t="n">
         <v>1000002</v>
       </c>
     </row>
-    <row r="32" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="32" t="s">
+    <row r="32" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C32" s="19" t="n">
+      <c r="C32" s="21" t="n">
         <f aca="false">(Sheet1!D32+Sheet1!E32)/Sheet1!F32</f>
         <v>0.00625</v>
       </c>
-      <c r="D32" s="13" t="n">
+      <c r="D32" s="15" t="n">
         <f aca="false">4*Sheet1!E32</f>
         <v>0.8</v>
       </c>
-      <c r="E32" s="13" t="n">
+      <c r="E32" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="F32" s="13" t="n">
+      <c r="F32" s="15" t="n">
         <v>160</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="I32" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J32" s="13" t="s">
+      <c r="J32" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="L32" s="19" t="n">
+      <c r="L32" s="21" t="n">
         <v>1000003</v>
       </c>
     </row>
-    <row r="33" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32" t="s">
+    <row r="33" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="19" t="n">
+      <c r="C33" s="21" t="n">
         <f aca="false">(Sheet1!D33+Sheet1!E33)/Sheet1!F33</f>
         <v>0.00625</v>
       </c>
-      <c r="D33" s="13" t="n">
+      <c r="D33" s="15" t="n">
         <f aca="false">4*Sheet1!E33</f>
         <v>0.8</v>
       </c>
-      <c r="E33" s="13" t="n">
+      <c r="E33" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="F33" s="13" t="n">
+      <c r="F33" s="15" t="n">
         <v>160</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="I33" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="L33" s="19" t="n">
+      <c r="L33" s="21" t="n">
         <v>1000004</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32" t="s">
+    <row r="34" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="C34" s="19" t="n">
+      <c r="C34" s="21" t="n">
         <f aca="false">(Sheet1!D34+Sheet1!E34)/Sheet1!F34</f>
         <v>0.00191607587660471</v>
       </c>
-      <c r="D34" s="13" t="n">
+      <c r="D34" s="15" t="n">
         <f aca="false">4*Sheet1!E34</f>
         <v>24</v>
       </c>
-      <c r="E34" s="13" t="n">
+      <c r="E34" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="F34" s="19" t="n">
+      <c r="F34" s="21" t="n">
         <v>15657</v>
       </c>
-      <c r="G34" s="19" t="n">
+      <c r="G34" s="21" t="n">
         <v>150.00075</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K34" s="13" t="s">
+      <c r="K34" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="L34" s="19" t="n">
+      <c r="L34" s="21" t="n">
         <v>1000005</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="32" t="s">
+    <row r="35" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="19" t="n">
+      <c r="C35" s="21" t="n">
         <f aca="false">(Sheet1!D35+Sheet1!E35)/Sheet1!F35</f>
         <v>0.00191082802547771</v>
       </c>
-      <c r="D35" s="13" t="n">
+      <c r="D35" s="15" t="n">
         <f aca="false">4*Sheet1!E35</f>
         <v>24</v>
       </c>
-      <c r="E35" s="13" t="n">
+      <c r="E35" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="F35" s="19" t="n">
+      <c r="F35" s="21" t="n">
         <v>15700</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13" t="s">
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="K35" s="13" t="s">
+      <c r="K35" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="L35" s="19" t="n">
+      <c r="L35" s="21" t="n">
         <v>1000006</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="33" t="s">
+    <row r="36" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="19" t="n">
+      <c r="C36" s="21" t="n">
         <f aca="false">(Sheet1!D36+Sheet1!E36)/Sheet1!F36</f>
         <v>0.0323974082073434</v>
       </c>
-      <c r="D36" s="13" t="n">
+      <c r="D36" s="15" t="n">
         <f aca="false">4*Sheet1!E36</f>
         <v>1.2</v>
       </c>
-      <c r="E36" s="13" t="n">
+      <c r="E36" s="15" t="n">
         <v>0.3</v>
       </c>
-      <c r="F36" s="19" t="n">
+      <c r="F36" s="21" t="n">
         <v>46.3</v>
       </c>
-      <c r="G36" s="19" t="n">
+      <c r="G36" s="21" t="n">
         <v>360.00252</v>
       </c>
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J36" s="13" t="s">
+      <c r="J36" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="L36" s="19" t="n">
+      <c r="K36" s="0"/>
+      <c r="L36" s="21" t="n">
         <v>1000007</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="33" t="s">
+    <row r="37" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="C37" s="19" t="n">
+      <c r="C37" s="21" t="n">
         <f aca="false">(Sheet1!D37+Sheet1!E37)/Sheet1!F37</f>
         <v>0.0323974082073434</v>
       </c>
-      <c r="D37" s="13" t="n">
+      <c r="D37" s="15" t="n">
         <f aca="false">4*Sheet1!E37</f>
         <v>1.2</v>
       </c>
-      <c r="E37" s="13" t="n">
+      <c r="E37" s="15" t="n">
         <v>0.3</v>
       </c>
-      <c r="F37" s="19" t="n">
+      <c r="F37" s="21" t="n">
         <v>46.3</v>
       </c>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13" t="s">
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="L37" s="19" t="n">
+      <c r="K37" s="0"/>
+      <c r="L37" s="21" t="n">
         <v>1000008</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="32" t="s">
+    <row r="38" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C38" s="19" t="n">
+      <c r="C38" s="21" t="n">
         <f aca="false">(Sheet1!D38+Sheet1!E38)/Sheet1!F38</f>
         <v>0.150375939849624</v>
       </c>
-      <c r="D38" s="13" t="n">
+      <c r="D38" s="15" t="n">
         <f aca="false">4*Sheet1!E38</f>
         <v>16</v>
       </c>
-      <c r="E38" s="13" t="n">
+      <c r="E38" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="F38" s="19" t="n">
+      <c r="F38" s="21" t="n">
         <v>133</v>
       </c>
-      <c r="G38" s="19" t="n">
+      <c r="G38" s="21" t="n">
         <v>15.000135</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="H38" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="I38" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="L38" s="19" t="n">
+      <c r="K38" s="0"/>
+      <c r="L38" s="21" t="n">
         <v>1000009</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="32" t="s">
+    <row r="39" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="C39" s="19" t="n">
+      <c r="C39" s="21" t="n">
         <f aca="false">(Sheet1!D39+Sheet1!E39)/Sheet1!F39</f>
         <v>0.150375939849624</v>
       </c>
-      <c r="D39" s="13" t="n">
+      <c r="D39" s="15" t="n">
         <f aca="false">4*Sheet1!E39</f>
         <v>16</v>
       </c>
-      <c r="E39" s="13" t="n">
+      <c r="E39" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="F39" s="19" t="n">
+      <c r="F39" s="21" t="n">
         <v>133</v>
       </c>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13" t="s">
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="J39" s="13" t="s">
+      <c r="J39" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="L39" s="19" t="n">
+      <c r="K39" s="0"/>
+      <c r="L39" s="21" t="n">
         <v>1000010</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
+      <c r="I40" s="0"/>
+      <c r="J40" s="0"/>
+      <c r="K40" s="0"/>
+      <c r="L40" s="0"/>
+    </row>
+    <row r="41" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
+      <c r="J41" s="0"/>
+      <c r="K41" s="0"/>
+      <c r="L41" s="0"/>
+    </row>
+    <row r="42" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B42" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="I42" s="0" t="s">
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
+      <c r="I42" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="J42" s="7" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+      <c r="K42" s="0"/>
+      <c r="L42" s="0"/>
+    </row>
+    <row r="43" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="I43" s="35" t="s">
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
+      <c r="I43" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="J43" s="0" t="s">
+      <c r="J43" s="7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I44" s="0" t="s">
+      <c r="K43" s="0"/>
+      <c r="L43" s="0"/>
+    </row>
+    <row r="44" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0"/>
+      <c r="H44" s="0"/>
+      <c r="I44" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="J44" s="0" t="s">
+      <c r="J44" s="7" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I45" s="36" t="s">
+      <c r="K44" s="0"/>
+      <c r="L44" s="0"/>
+    </row>
+    <row r="45" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="G45" s="0"/>
+      <c r="H45" s="0"/>
+      <c r="I45" s="37" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J45" s="0"/>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
+    </row>
+    <row r="46" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
+      <c r="F46" s="0"/>
+      <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="J46" s="0"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="C47" s="23" t="n">
+      <c r="C47" s="25" t="n">
         <v>0.06</v>
       </c>
-      <c r="D47" s="12" t="n">
+      <c r="D47" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="23" t="n">
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="25" t="n">
         <v>100</v>
       </c>
-      <c r="H47" s="12"/>
-      <c r="I47" s="37" t="s">
+      <c r="H47" s="14"/>
+      <c r="I47" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="J47" s="0" t="s">
+      <c r="J47" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="38" t="s">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12" t="n">
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="I48" s="37" t="s">
+      <c r="I48" s="38" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="38" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C49" s="12" t="n">
+      <c r="C49" s="14" t="n">
         <f aca="false">(Sheet1!D49+Sheet1!E49)/Sheet1!F49</f>
         <v>0.000198000198000198</v>
       </c>
-      <c r="D49" s="12" t="n">
+      <c r="D49" s="14" t="n">
         <v>0.08</v>
       </c>
-      <c r="E49" s="12" t="n">
+      <c r="E49" s="14" t="n">
         <v>0.02</v>
       </c>
-      <c r="F49" s="23" t="n">
+      <c r="F49" s="25" t="n">
         <v>505.05</v>
       </c>
-      <c r="G49" s="23" t="n">
+      <c r="G49" s="25" t="n">
         <v>500</v>
       </c>
-      <c r="H49" s="12" t="n">
+      <c r="H49" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="I49" s="0" t="s">
+      <c r="I49" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-    </row>
-    <row r="51" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="C51" s="8" t="n">
+      <c r="C51" s="10" t="n">
         <v>0.02</v>
       </c>
-      <c r="D51" s="8" t="n">
+      <c r="D51" s="10" t="n">
         <v>6.4</v>
       </c>
-      <c r="E51" s="8" t="n">
+      <c r="E51" s="10" t="n">
         <v>1.6</v>
       </c>
-      <c r="G51" s="8" t="n">
+      <c r="F51" s="12" t="n">
+        <f aca="false">(D51+E51)/C51</f>
+        <v>400</v>
+      </c>
+      <c r="G51" s="10" t="n">
         <v>140</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="I51" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J51" s="8" t="s">
+      <c r="J51" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="L51" s="8" t="s">
+      <c r="L51" s="10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="52" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="s">
+    <row r="52" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="I52" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="K52" s="10"/>
-    </row>
-    <row r="53" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10"/>
-      <c r="I53" s="8" t="s">
+      <c r="J52" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="K53" s="10"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="s">
+      <c r="L52" s="10"/>
+    </row>
+    <row r="53" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="B55" s="39" t="s">
+      <c r="I53" s="10" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
+      <c r="K53" s="12"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="55" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="K55" s="12"/>
+    </row>
+    <row r="56" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K56" s="12"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6"/>
+      <c r="B58" s="40"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="0" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3841,188 +3995,185 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="F1" s="0" t="n">
         <v>0.418</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0.0368</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>12.7</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>7050</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>1310</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0.0525</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>57.4</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>77</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0.2</v>
@@ -4034,21 +4185,21 @@
         <v>200</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="K10" s="40" t="s">
-        <v>235</v>
+        <v>239</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>5</v>
@@ -4057,24 +4208,24 @@
         <v>50</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="K11" s="41" t="s">
-        <v>237</v>
+        <v>239</v>
+      </c>
+      <c r="K11" s="42" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>238</v>
+        <v>199</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>243</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>130</v>
@@ -4083,84 +4234,84 @@
         <v>200</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="K12" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
+      </c>
+      <c r="K12" s="44" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>100</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>100</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>50</v>
@@ -4169,86 +4320,86 @@
         <v>380</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>0.01</v>
@@ -4263,12 +4414,12 @@
         <v>180</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>0.014</v>
@@ -4283,12 +4434,12 @@
         <v>180</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>0.0029</v>
@@ -4303,7 +4454,7 @@
         <v>180</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates were made, new reactions added, morphology modified.  Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/ErkParams.xlsx
+++ b/ErkParams.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="kdiff" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="266">
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">values we are using</t>
+  </si>
   <si>
     <t xml:space="preserve">species id</t>
   </si>
@@ -75,9 +81,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
     <t xml:space="preserve">More notes</t>
   </si>
   <si>
@@ -136,6 +139,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Membrane molecule</t>
+  </si>
+  <si>
     <t xml:space="preserve">RasGRF</t>
   </si>
   <si>
@@ -526,6 +532,183 @@
     <t xml:space="preserve">Km=0.01 uM = 10 nM Vmax=0.024/sec ; Tsalkova PNAS 2013.  Rehmann JBC 278:23508 ; Rap1 conc=0.2 uM  = 200 nM from Sasagawa</t>
   </si>
   <si>
+    <t xml:space="preserve">Rap activates bRaf ??</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rap1GTP +</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rap1GAP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;-&gt; Rap1GTP.Gap --&gt; Rap1Gap+Rap1GDP</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0.012 uM = 12 nM, Km=1 uM=1000 nM Vmax=2/sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PKA to Rap1 via Src/Cbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PKA activation of Src</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PKAc +</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;-&gt; PKAc_Src -&gt; PKAc + pSrc</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Jain and Bhalla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRENDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity assumed, check Km and kcat; Schmidt and Stork J Biol Chem #277 p 43024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inact Src</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pSrc -&gt; Src</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activate Cbl</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Cbl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + pSrc &lt;-&gt; Cbl_pSrc&lt;-&gt;pCbl + pSrc</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sasagawa for quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inactivate Cbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pCbl&lt;=&gt; Cbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sasagawa Nat Cell Biol </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activate Crk, step1??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRK + C3G &lt;=&gt; CRK_C3G </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000, 500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sasagawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not needed? Hu CD,et al. (1999) Effect of phosphorylation on activities of Rap1A to interact with Raf-1 and to suppress Ras-dependent Raf-1 activation. J Biol Chem 274:48–51.  Normally CRK and C3G are complexed together</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activae Crk, step2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRK_C3G + pCbl &lt;=&gt; CRK_C3G_pCbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rap activation by Crk (GEF)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rap1GDP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ CRK_C3G_pCbl&lt;-&gt;CRK_C3G_pCbl_Rap1 -&gt; Rap1GTP + CRK_C3G_pCbl</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">same quant as ode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inactivation of Rap1 without Gap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rap1GTP  --&gt; Rap1GDP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inactivation of Rap1</t>
   </si>
   <si>
@@ -555,27 +738,42 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">&lt;-&gt; Rap1GTP.Gap --&gt; Rap1Gap+Rap1</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">0.012 uM = 12 nM, Km=1 uM=1000 nM Vmax=2/sec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PKA to Rap1 via Src/Cbl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PKA activation of Src</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PKAc +</t>
+      <t xml:space="preserve">&lt;-&gt; Rap1GTPGap --&gt; Rap1Gap+Rap1GDP</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">same quant, but lower affinity than ode file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PKA phos Rap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PKA + Rap1GDP &lt;-&gt; PKA + pRap1GDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vossler Cell 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pRap1 binds bRaf? Or pRap1 acquires GTP without GEF? Or enhances Rap1 or Ras binding?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Brenda for rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rap/Ras activation of Mapk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed in Orton Biochem J</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rap1GTP+</t>
     </r>
     <r>
       <rPr>
@@ -585,37 +783,43 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;-&gt; PKAc_Src -&gt; PKAc + pSrc</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Jain and Bhalla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRENDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity assumed, check Km and kcat; Schmidt and Stork J Biol Chem #277 p 43024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inact Src</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pSrc -&gt; Src</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activate Cbl</t>
-  </si>
-  <si>
+      <t xml:space="preserve">bRaf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;-&gt; bRafRap1GTP</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Jain and Bhalla PLoS One Suppl 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ras activates bRaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RasGTP+bRaf &lt;-&gt; bRafRasGTP **</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other source: Buhrman G, Senthil Kumar VS, Cirit M, Haugh JM, Mattos C (2011) Allosteric modulation of Ras-GTP is linked to signal transduction through RAF kinase. J Biol Chem 286: 3323–3331. doi:10.1074/jbc.M110.193854.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inactivation of Raf-Rap1GTP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bRafRap1GTP +</t>
+    </r>
     <r>
       <rPr>
         <b val="true"/>
@@ -624,53 +828,23 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Cbl</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> + pSrc &lt;-&gt; Cbl_pSrc&lt;-&gt;pCbl + pSrc</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Sasagawa for quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inactivate Cbl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pCbl&lt;=&gt; Cbl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sasagawa Nat Cell Biol </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activate Crk, step1??</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRK + C3G &lt;=&gt; CRK_C3G </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000, 500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sasagawa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not needed? Hu CD,et al. (1999) Effect of phosphorylation on activities of Rap1A to interact with Raf-1 and to suppress Ras-dependent Raf-1 activation. J Biol Chem 274:48–51.  Normally CRK and C3G are complexed together</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activae Crk, step2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRK_C3G + pCbl &lt;=&gt; CRK_C3G_pCbl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rap activation by Crk (GEF)</t>
+      <t xml:space="preserve">Rap1Gap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;-&gt; bRaf_Rap1GTP_RapGap --&gt; bRaf+Rap1Gap+Rap1GDP</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">***MEK=MAPKK, ERK=MAPK, Raf=MAPKKK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPKK phos1 by bRaf-Rap1</t>
   </si>
   <si>
     <r>
@@ -681,36 +855,67 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Rap1GDP </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ CRK_C3G_pCbl&lt;-&gt;CRK_C3G_pCbl_Rap1 -&gt; Rap1GTP + CRK_C3G_pCbl</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">same quant as ode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inactivation of Rap1 without Gap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rap1GTP  --&gt; Rap1GDP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rap1GTP +</t>
+      <t xml:space="preserve">MAPKK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + bRafRap1GTP &lt;-&gt; bRafRap1GTPMAPKK &lt;-&gt; pMAPKK + bRafRap1GTP</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPKK phos2  by bRaf-Rap1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pMAPKK + bRaf_Rap1GTP &lt;-&gt; BRafRap1GTPpMAPKK &lt;-&gt; ppMAPKK + bRaf_Rap1GTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPKK phos1 by bRaf-Ras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPKK + bRafRasGTP &lt;-&gt; bRafRasGTPMAPKK &lt;-&gt; pMAPKK+ bRafRasGTP**</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF5B9BD5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAPKK phos2  by bRaf-Ra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFED7D31"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">s</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">pMAPKK + bRafRasGTP &lt;-&gt; bRafRasGTPpMAPKK&lt;-&gt; ppMAPKK + bRafRasGTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppMAPKK dephos1 by PP2A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ppMAPKK+</t>
     </r>
     <r>
       <rPr>
@@ -720,54 +925,64 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Rap1GAP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;-&gt; Rap1GTPGap --&gt; Rap1Gap+Rap1GDP</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">same quant, but lower affinity than ode file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PKA phos Rap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PKA + Rap1GDP &lt;-&gt; PKA + pRap1GDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vossler Cell 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pRap1 binds bRaf? Or pRap1 acquires GTP without GEF? Or enhances Rap1 or Ras binding?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Brenda for rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rap/Ras activation of Mapk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewed in Orton Biochem J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rap activates bRaf ??</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rap1GTP+</t>
+      <t xml:space="preserve">PP2A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;-&gt;ppMAPKKPP2A &lt;-&gt; pMAPKK+PP2A</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">nonzero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These phos steps are barely cooperative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppMAPKK dephos2 by PP2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pMAPKK+PP2A &lt;-&gt; pMAPKKPP2A &lt;-&gt; MAPKK+PP2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other source: Letourneux C, Rocher G, Porteu F (2006) B56-containing PP2A dephosphorylate ERK and their activity is controlled by the early gene IEX-1 and ERK. EMBO J 25: 727–738. doi:10.1038/sj.emboj.7600980; Zhou B, Wang Z-X, Zhao Y, Brautigan DL, Zhang Z-Y (2002) The specificity of extracellular signal-regulated kinase 2 dephosphorylation by protein phosphatases. J Biol Chem 277: 31818–31825. doi:10.1074/jbc.M203969200.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFED7D31"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ERK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF5B9BD5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> phos1 by ppMAPKK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ppMAPKK+</t>
     </r>
     <r>
       <rPr>
@@ -777,42 +992,58 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">bRaf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;-&gt; bRafRap1GTP</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Jain and Bhalla PLoS One Suppl 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ras activates bRaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RasGTP+bRaf &lt;-&gt; bRafRasGTP **</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other source: Buhrman G, Senthil Kumar VS, Cirit M, Haugh JM, Mattos C (2011) Allosteric modulation of Ras-GTP is linked to signal transduction through RAF kinase. J Biol Chem 286: 3323–3331. doi:10.1074/jbc.M110.193854.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inactivation of Raf-Rap1GTP</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">bRafRap1GTP +</t>
+      <t xml:space="preserve">ERK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;-&gt; ppMAPKKERK &lt;-&gt; pERK+ppMAPKK</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DOCQS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFED7D31"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ERK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF5B9BD5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (1) phos2 by ppMAPKK</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ppMAPKK+pERK&lt;-&gt;ppMAPKKpERK &lt;-&gt;ppERK+ppMAPKK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppERK dephos1 by MKP1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ppERK+</t>
     </r>
     <r>
       <rPr>
@@ -822,23 +1053,26 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Rap1Gap</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;-&gt; bRaf_Rap1GTP_RapGap --&gt; bRaf+Rap1Gap+Rap1GDP</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">***MEK=MAPKK, ERK=MAPK, Raf=MAPKKK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAPKK phos1 by bRaf-Rap1</t>
+      <t xml:space="preserve">MKP1&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-&gt; ppERKMKP1 &lt;-&gt; pERK+MKP1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ppERK dephos2 by MKP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pERK+MKP1&lt;-&gt; pERKMKP1 &lt;-&gt; ERK+MKP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bAR recruitment of arrestin</t>
   </si>
   <si>
     <r>
@@ -849,67 +1083,33 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">MAPKK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> + bRafRap1GTP &lt;-&gt; bRafRap1GTPMAPKK &lt;-&gt; pMAPKK + bRafRap1GTP</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">MAPKK phos2  by bRaf-Rap1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pMAPKK + bRaf_Rap1GTP &lt;-&gt; BRafRap1GTPpMAPKK &lt;-&gt; ppMAPKK + bRaf_Rap1GTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAPKK phos1 by bRaf-Ras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAPKK + bRafRasGTP &lt;-&gt; bRafRasGTPMAPKK &lt;-&gt; pMAPKK+ bRafRasGTP**</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MAPKK phos2  by bRaf-Ra</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFED7D31"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">s</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">pMAPKK + bRafRasGTP &lt;-&gt; bRafRasGTPpMAPKK&lt;-&gt; ppMAPKK + bRafRasGTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ppMAPKK dephos1 by PP2A</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ppMAPKK+</t>
+      <t xml:space="preserve">Grk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+NE-bAR &lt;-&gt; Grk+pbAR</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> 75=shenoy ... Lefkowitz JBC paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b-arrestin recruits Raf, MEK and ERK to the receptor</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">pbAR+</t>
     </r>
     <r>
       <rPr>
@@ -919,64 +1119,48 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">PP2A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;-&gt;ppMAPKKPP2A &lt;-&gt; pMAPKK+PP2A</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">nonzero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These phos steps are barely cooperative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ppMAPKK dephos2 by PP2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pMAPKK+PP2A &lt;-&gt; pMAPKKPP2A &lt;-&gt; MAPKK+PP2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other source: Letourneux C, Rocher G, Porteu F (2006) B56-containing PP2A dephosphorylate ERK and their activity is controlled by the early gene IEX-1 and ERK. EMBO J 25: 727–738. doi:10.1038/sj.emboj.7600980; Zhou B, Wang Z-X, Zhao Y, Brautigan DL, Zhang Z-Y (2002) The specificity of extracellular signal-regulated kinase 2 dephosphorylation by protein phosphatases. J Biol Chem 277: 31818–31825. doi:10.1074/jbc.M203969200.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFED7D31"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ERK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> phos1 by ppMAPKK</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ppMAPKK+</t>
+      <t xml:space="preserve">arr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;-&gt; bpAR-arr-+Raf+Mek+erk</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Heitzler,D. et al. Competing G protein-coupled receptor kinases balance G protein and beta-arrestin signaling. Mol. Syst. Biol. 8, 590 (2012).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ß2-adrenergic activation of MEK/ERK cascade  two separate components: a rapid, transient signal that peaks 2–5 min after stimulation, and a slower but more sustained signal peaking 5–10 min after stimulation, but lasting for nearly 30 min [75].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahn Lefkowitz JBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The early ERK activation is dependant on GPCR and protein kinase A (PKA) but is completely independent of ß-arrestin. the delayed response is independent of GPCR and PKA, but requires ß-arrestin and can be inhibited by siRNA knockdown of ß-arrestin [75].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vayttaden - bAR cycling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CaCam activation of Ras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activaton of RasGRF (GEF) (inact-GEF?)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CamCa4+</t>
     </r>
     <r>
       <rPr>
@@ -986,58 +1170,42 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">ERK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;-&gt; ppMAPKKERK &lt;-&gt; pERK+ppMAPKK</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">DOCQS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFED7D31"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ERK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (1) phos2 by ppMAPKK</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ppMAPKK+pERK&lt;-&gt;ppMAPKKpERK &lt;-&gt;ppERK+ppMAPKK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ppERK dephos1 by MKP1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ppERK+</t>
+      <t xml:space="preserve">RasGRF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;-&gt; RasGRF_CamCa4</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Farnsworth, C. L., N. W. Freshney, L. B. Rosen, A. Ghosh, M. E. Greenberg, and L. A. Felg. 1995. Calcium activation of Ras mediated by neuronal exchange factor Ras-GRF. Nature 376:524–527; Ras increases from 19% (basal) to 42% (calcium), but not in RasGRF-IQ mutants.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gutierrez-Arenas (Kotaleski) PLoS Comp Biol 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activaton of RasGRF (GEF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jin, Feig JBC VOL. 289, NO. 23, pp. 16551–16564,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active RasGRF activates Ras</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RasGRF_CamCa4 +</t>
     </r>
     <r>
       <rPr>
@@ -1047,168 +1215,6 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">MKP1&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-&gt; ppERKMKP1 &lt;-&gt; pERK+MKP1</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ppERK dephos2 by MKP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pERK+MKP1&lt;-&gt; pERKMKP1 &lt;-&gt; ERK+MKP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bAR recruitment of arrestin</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Grk</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+NE-bAR &lt;-&gt; Grk+pbAR</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> 75=shenoy ... Lefkowitz JBC paper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b-arrestin recruits Raf, MEK and ERK to the receptor</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">pbAR+</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">arr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;-&gt; bpAR-arr-+Raf+Mek+erk</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Heitzler,D. et al. Competing G protein-coupled receptor kinases balance G protein and beta-arrestin signaling. Mol. Syst. Biol. 8, 590 (2012).</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ß2-adrenergic activation of MEK/ERK cascade  two separate components: a rapid, transient signal that peaks 2–5 min after stimulation, and a slower but more sustained signal peaking 5–10 min after stimulation, but lasting for nearly 30 min [75].</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ahn Lefkowitz JBC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The early ERK activation is dependant on GPCR and protein kinase A (PKA) but is completely independent of ß-arrestin. the delayed response is independent of GPCR and PKA, but requires ß-arrestin and can be inhibited by siRNA knockdown of ß-arrestin [75].</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vayttaden - bAR cycling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaCam activation of Ras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activaton of RasGRF (GEF) (inact-GEF?)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CamCa4+</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">RasGRF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;-&gt; RasGRF_CamCa4</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Farnsworth, C. L., N. W. Freshney, L. B. Rosen, A. Ghosh, M. E. Greenberg, and L. A. Felg. 1995. Calcium activation of Ras mediated by neuronal exchange factor Ras-GRF. Nature 376:524–527; Ras increases from 19% (basal) to 42% (calcium), but not in RasGRF-IQ mutants.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gutierrez-Arenas (Kotaleski) PLoS Comp Biol 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activaton of RasGRF (GEF)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jin, Feig JBC VOL. 289, NO. 23, pp. 16551–16564,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">active RasGRF activates Ras</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">RasGRF_CamCa4 +</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve">RasGDP</t>
     </r>
     <r>
@@ -1231,13 +1237,16 @@
     <t xml:space="preserve">Km=1 uM=1000 nM Vmax=10/sec;  This catalytic rate assumes that pDok is bound</t>
   </si>
   <si>
+    <t xml:space="preserve">J Biol Chem. 2015 Feb 20;290(8):4908-27.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From table 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inactivation of Rap</t>
   </si>
   <si>
-    <t xml:space="preserve">RapGTP +SynGAP&lt;-&gt; RapGTP.Gap --&gt; SynGap+Rap(GDP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J Biol Chem. 2015 Feb 20;290(8):4908-27.</t>
+    <t xml:space="preserve">Rap1GTP +SynGAP&lt;-&gt; Rap1GTP.Gap --&gt; SynGap+Rap1(GDP)</t>
   </si>
   <si>
     <t xml:space="preserve">Interpreted from figures</t>
@@ -1246,43 +1255,16 @@
     <t xml:space="preserve">RasGTP +pSynGAP&lt;-&gt; RasGTP.Gap --&gt; pSynGap+Ras(GDP)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Walkup WG 4th, Washburn L, Sweredoski MJ, Carlisle HJ, Graham RL, Hess S, </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Kennedy MB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RapGTP +pSynGAP&lt;-&gt; RapGTP.Gap --&gt; pSynGap+Rap(GDP)</t>
+    <t xml:space="preserve">Rap1GTP +pSynGAP&lt;-&gt; Rap1GTP.Gap --&gt; pSynGap+Rap1(GDP)</t>
   </si>
   <si>
     <t xml:space="preserve">CaMKII inhib SynGap</t>
   </si>
   <si>
     <t xml:space="preserve">CKpCamCa4+SynGap &lt;-&gt; CKpCamCa4+pSynGap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walkup WG 4th, Washburn L, Sweredoski MJ, Carlisle HJ, Graham RL, Hess S, Kennedy MB.</t>
   </si>
   <si>
     <t xml:space="preserve">Calmodulin working through Pyk2</t>
@@ -2119,22 +2101,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="158.479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="67.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="156.724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2147,430 +2129,532 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="E19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0.836</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="0" t="n">
         <v>0.6</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="n">
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="0" t="n">
         <v>0.6</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>86.4</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" s="2" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>0.836</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>86.4</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="0" t="n">
+      <c r="E50" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="0" t="n">
         <v>0.6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2599858/ "/>
-    <hyperlink ref="C24" r:id="rId2" display="http://www.cell.com/cms/attachment/2021781245/2041678471/mmc1.pdf says 0"/>
-    <hyperlink ref="D49" r:id="rId3" display="different values according to https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2908681/"/>
-    <hyperlink ref="C50" r:id="rId4" display="Epac1camp is 10 from here: https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4763502/"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2599858/ "/>
+    <hyperlink ref="E24" r:id="rId2" display="http://www.cell.com/cms/attachment/2021781245/2041678471/mmc1.pdf says 0"/>
+    <hyperlink ref="F49" r:id="rId3" display="different values according to https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2908681/"/>
+    <hyperlink ref="E50" r:id="rId4" display="Epac1camp is 10 from here: https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4763502/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -2587,71 +2671,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1530" topLeftCell="A37" activePane="bottomLeft" state="split"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1530" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="48.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="47.6530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C2" s="10" t="n">
         <v>0.0002</v>
@@ -2663,21 +2745,21 @@
         <v>200</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C3" s="10" t="n">
         <v>0.08</v>
@@ -2692,41 +2774,41 @@
         <v>100</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>1.28</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>0.48</v>
@@ -2741,15 +2823,15 @@
         <v>100</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2761,7 +2843,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -2774,10 +2856,10 @@
     </row>
     <row r="8" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C8" s="17" t="n">
         <v>0.000234</v>
@@ -2792,18 +2874,18 @@
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C9" s="15" t="n">
         <v>0.012</v>
@@ -2820,18 +2902,18 @@
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C10" s="15" t="n">
         <f aca="false">0.04</f>
@@ -2851,10 +2933,10 @@
         <v>12</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +2951,7 @@
     </row>
     <row r="12" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -2882,10 +2964,10 @@
     </row>
     <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C13" s="21" t="n">
         <f aca="false">(Sheet1!D13+Sheet1!E13)/Sheet1!F13</f>
@@ -2907,21 +2989,21 @@
         <v>0</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C14" s="15" t="n">
         <v>100</v>
@@ -2934,15 +3016,15 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C15" s="15" t="n">
         <f aca="false">(Sheet1!D15+Sheet1!E15)/Sheet1!F15</f>
@@ -2964,21 +3046,21 @@
         <v>0</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C16" s="15" t="n">
         <v>10</v>
@@ -2991,18 +3073,18 @@
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>0.001</v>
@@ -3013,27 +3095,27 @@
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H17" s="15" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C18" s="15" t="n">
         <v>0.001</v>
@@ -3048,15 +3130,15 @@
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C19" s="21" t="n">
         <f aca="false">(Sheet1!D19+Sheet1!E19)/Sheet1!F19</f>
@@ -3078,21 +3160,21 @@
         <v>0</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C20" s="15" t="n">
         <v>0.0001</v>
@@ -3105,18 +3187,18 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C21" s="21" t="n">
         <f aca="false">(Sheet1!D21+Sheet1!E21)/Sheet1!F21</f>
@@ -3138,13 +3220,13 @@
         <v>0</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,10 +3241,10 @@
     </row>
     <row r="23" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -3171,12 +3253,12 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="23" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="10" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -3185,7 +3267,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3200,7 +3282,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -3211,15 +3293,15 @@
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="K26" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C27" s="25" t="n">
         <v>0.06</v>
@@ -3236,18 +3318,18 @@
         <v>0</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C28" s="26" t="n">
         <v>0.06</v>
@@ -3259,21 +3341,21 @@
         <v>200</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C29" s="28" t="n">
         <f aca="false">(Sheet1!D29+Sheet1!E29)/Sheet1!F29</f>
@@ -3295,13 +3377,13 @@
         <v>0</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="L29" s="29" t="n">
         <v>1000000</v>
@@ -3309,10 +3391,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C30" s="28" t="n">
         <f aca="false">(Sheet1!D30+Sheet1!E30)/Sheet1!F30</f>
@@ -3335,10 +3417,10 @@
         <v>0</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L30" s="29" t="n">
         <v>1000001</v>
@@ -3346,10 +3428,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C31" s="28" t="n">
         <f aca="false">(Sheet1!D31+Sheet1!E31)/Sheet1!F31</f>
@@ -3368,10 +3450,10 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L31" s="29" t="n">
         <v>1000002</v>
@@ -3379,10 +3461,10 @@
     </row>
     <row r="32" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="33" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C32" s="21" t="n">
         <f aca="false">(Sheet1!D32+Sheet1!E32)/Sheet1!F32</f>
@@ -3399,10 +3481,10 @@
         <v>160</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L32" s="21" t="n">
         <v>1000003</v>
@@ -3410,10 +3492,10 @@
     </row>
     <row r="33" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="33" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C33" s="21" t="n">
         <f aca="false">(Sheet1!D33+Sheet1!E33)/Sheet1!F33</f>
@@ -3430,10 +3512,10 @@
         <v>160</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L33" s="21" t="n">
         <v>1000004</v>
@@ -3441,10 +3523,10 @@
     </row>
     <row r="34" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="33" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C34" s="21" t="n">
         <f aca="false">(Sheet1!D34+Sheet1!E34)/Sheet1!F34</f>
@@ -3464,27 +3546,27 @@
         <v>150.00075</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="L34" s="21" t="n">
         <v>1000005</v>
       </c>
     </row>
-    <row r="35" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="33" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C35" s="21" t="n">
         <f aca="false">(Sheet1!D35+Sheet1!E35)/Sheet1!F35</f>
@@ -3503,24 +3585,24 @@
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L35" s="21" t="n">
         <v>1000006</v>
       </c>
     </row>
-    <row r="36" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="34" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C36" s="21" t="n">
         <f aca="false">(Sheet1!D36+Sheet1!E36)/Sheet1!F36</f>
@@ -3540,25 +3622,24 @@
         <v>360.00252</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="K36" s="0"/>
+        <v>161</v>
+      </c>
       <c r="L36" s="21" t="n">
         <v>1000007</v>
       </c>
     </row>
-    <row r="37" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="34" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C37" s="21" t="n">
         <f aca="false">(Sheet1!D37+Sheet1!E37)/Sheet1!F37</f>
@@ -3577,22 +3658,21 @@
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="K37" s="0"/>
+        <v>161</v>
+      </c>
       <c r="L37" s="21" t="n">
         <v>1000008</v>
       </c>
     </row>
-    <row r="38" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="33" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C38" s="21" t="n">
         <f aca="false">(Sheet1!D38+Sheet1!E38)/Sheet1!F38</f>
@@ -3612,25 +3692,24 @@
         <v>15.000135</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="K38" s="0"/>
+        <v>161</v>
+      </c>
       <c r="L38" s="21" t="n">
         <v>1000009</v>
       </c>
     </row>
-    <row r="39" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="33" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C39" s="21" t="n">
         <f aca="false">(Sheet1!D39+Sheet1!E39)/Sheet1!F39</f>
@@ -3649,142 +3728,64 @@
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="K39" s="0"/>
+        <v>161</v>
+      </c>
       <c r="L39" s="21" t="n">
         <v>1000010</v>
       </c>
     </row>
-    <row r="40" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
-      <c r="F40" s="0"/>
-      <c r="G40" s="0"/>
-      <c r="H40" s="0"/>
-      <c r="I40" s="0"/>
-      <c r="J40" s="0"/>
-      <c r="K40" s="0"/>
-      <c r="L40" s="0"/>
-    </row>
-    <row r="41" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
-      <c r="D41" s="0"/>
-      <c r="E41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
-      <c r="H41" s="0"/>
-      <c r="I41" s="0"/>
-      <c r="J41" s="0"/>
-      <c r="K41" s="0"/>
-      <c r="L41" s="0"/>
-    </row>
-    <row r="42" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="C42" s="0"/>
-      <c r="D42" s="0"/>
-      <c r="E42" s="0"/>
-      <c r="F42" s="0"/>
-      <c r="G42" s="0"/>
-      <c r="H42" s="0"/>
+        <v>169</v>
+      </c>
       <c r="I42" s="7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K42" s="0"/>
-      <c r="L42" s="0"/>
-    </row>
-    <row r="43" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C43" s="0"/>
-      <c r="D43" s="0"/>
-      <c r="E43" s="0"/>
-      <c r="F43" s="0"/>
-      <c r="G43" s="0"/>
-      <c r="H43" s="0"/>
+        <v>172</v>
+      </c>
       <c r="I43" s="36" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="K43" s="0"/>
-      <c r="L43" s="0"/>
-    </row>
-    <row r="44" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
-      <c r="D44" s="0"/>
-      <c r="E44" s="0"/>
-      <c r="F44" s="0"/>
-      <c r="G44" s="0"/>
-      <c r="H44" s="0"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I44" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="K44" s="0"/>
-      <c r="L44" s="0"/>
-    </row>
-    <row r="45" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="B45" s="0"/>
-      <c r="C45" s="0"/>
-      <c r="D45" s="0"/>
-      <c r="E45" s="0"/>
-      <c r="F45" s="0"/>
-      <c r="G45" s="0"/>
-      <c r="H45" s="0"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I45" s="37" t="s">
-        <v>175</v>
-      </c>
-      <c r="J45" s="0"/>
-      <c r="K45" s="0"/>
-      <c r="L45" s="0"/>
-    </row>
-    <row r="46" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
-      <c r="E46" s="0"/>
-      <c r="F46" s="0"/>
-      <c r="G46" s="0"/>
-      <c r="H46" s="0"/>
-      <c r="I46" s="0"/>
-      <c r="J46" s="0"/>
-      <c r="K46" s="0"/>
-      <c r="L46" s="0"/>
+        <v>178</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C47" s="25" t="n">
         <v>0.06</v>
@@ -3799,18 +3800,18 @@
       </c>
       <c r="H47" s="14"/>
       <c r="I47" s="38" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
@@ -3821,15 +3822,15 @@
         <v>0</v>
       </c>
       <c r="I48" s="38" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="39" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C49" s="14" t="n">
         <f aca="false">(Sheet1!D49+Sheet1!E49)/Sheet1!F49</f>
@@ -3851,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,10 +3866,10 @@
     </row>
     <row r="51" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C51" s="10" t="n">
         <v>0.02</v>
@@ -3887,89 +3888,118 @@
         <v>140</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
+      <c r="E52" s="10" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="F52" s="12" t="n">
+        <v>640000</v>
+      </c>
       <c r="G52" s="10"/>
       <c r="I52" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="J52" s="10" t="s">
+      <c r="J52" s="10"/>
+      <c r="K52" s="12" t="s">
         <v>191</v>
       </c>
       <c r="L52" s="10"/>
     </row>
-    <row r="53" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B53" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="0"/>
+      <c r="G53" s="10"/>
+      <c r="I53" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="L53" s="10"/>
+    </row>
+    <row r="54" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I54" s="10"/>
+      <c r="K54" s="12"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="I53" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="K53" s="12"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="55" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="I55" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="K55" s="12"/>
     </row>
     <row r="56" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="K56" s="12"/>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B57" s="40" t="s">
-        <v>198</v>
-      </c>
+    <row r="57" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0"/>
+      <c r="B57" s="0"/>
+      <c r="I57" s="0"/>
+      <c r="K57" s="12"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6"/>
-      <c r="B58" s="40"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
-        <v>87</v>
+      <c r="A58" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B58" s="40" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="6"/>
+      <c r="B59" s="40"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3995,185 +4025,188 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F1" s="0" t="n">
         <v>0.418</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0.0368</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>12.7</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>7050</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>1310</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0.0525</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>57.4</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>77</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0.2</v>
@@ -4185,21 +4218,21 @@
         <v>200</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="K10" s="41" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>5</v>
@@ -4208,24 +4241,24 @@
         <v>50</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>130</v>
@@ -4234,84 +4267,84 @@
         <v>200</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="K12" s="44" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>100</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>100</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>50</v>
@@ -4320,86 +4353,86 @@
         <v>380</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>0.01</v>
@@ -4411,15 +4444,15 @@
         <v>0.6</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>0.014</v>
@@ -4431,15 +4464,15 @@
         <v>10</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>0.0029</v>
@@ -4451,10 +4484,10 @@
         <v>8</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed rate values for camca4+RasGRF rxn in rxn file and ERKparams spreadsheet, added a results sheet to the spreadsheet, ongoing changes to stimtest file as per simulations.
</commit_message>
<xml_diff>
--- a/ErkParams.xlsx
+++ b/ErkParams.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="kdiff" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Rxns and rates" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Unused rxns" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Understanding rxns" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Results" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="369">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -1885,6 +1886,21 @@
   <si>
     <t xml:space="preserve">ppERK+MKP1&lt;-&gt; ppERKMKP1 &lt;-&gt; pERK+MKP1</t>
   </si>
+  <si>
+    <t xml:space="preserve">Peakval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CamCa4 (rate molecules/ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cAMP (rate molecules/ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T/2 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cAMP</t>
+  </si>
 </sst>
 </file>
 
@@ -1895,7 +1911,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
     <numFmt numFmtId="166" formatCode="0.00E+000"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2054,6 +2070,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -2117,7 +2139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -2130,6 +2152,13 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="double"/>
+      <right style="double"/>
+      <top style="double"/>
+      <bottom style="double"/>
       <diagonal/>
     </border>
   </borders>
@@ -2158,7 +2187,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2399,6 +2428,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -3204,7 +3253,7 @@
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1530" topLeftCell="A34" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I56" activeCellId="0" sqref="I56"/>
+      <selection pane="bottomLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4286,7 +4335,7 @@
         <v>177</v>
       </c>
       <c r="C47" s="16" t="n">
-        <v>0.006</v>
+        <v>0.06</v>
       </c>
       <c r="D47" s="11" t="n">
         <v>1</v>
@@ -4294,7 +4343,7 @@
       <c r="E47" s="11"/>
       <c r="F47" s="11" t="n">
         <f aca="false">D47/C47</f>
-        <v>166.666666666667</v>
+        <v>16.6666666666667</v>
       </c>
       <c r="G47" s="16" t="n">
         <v>100</v>
@@ -5240,7 +5289,7 @@
   </sheetPr>
   <dimension ref="1:57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -56785,4 +56834,522 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="22.05"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="60" width="13.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="60" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="61" t="s">
+        <v>364</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+    </row>
+    <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="61" t="s">
+        <v>365</v>
+      </c>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+    </row>
+    <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="64" t="s">
+        <v>366</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="62" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" s="62" t="n">
+        <v>200</v>
+      </c>
+      <c r="F3" s="62" t="n">
+        <v>600</v>
+      </c>
+      <c r="G3" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H3" s="62" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I3" s="62" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J3" s="62" t="n">
+        <v>20000</v>
+      </c>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+    </row>
+    <row r="4" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="64"/>
+      <c r="B4" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62" t="n">
+        <v>14.71</v>
+      </c>
+      <c r="F4" s="62" t="n">
+        <v>20.53</v>
+      </c>
+      <c r="G4" s="62" t="n">
+        <v>22.21</v>
+      </c>
+      <c r="H4" s="62" t="n">
+        <v>22.33</v>
+      </c>
+      <c r="I4" s="62" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="J4" s="62" t="n">
+        <v>23.86</v>
+      </c>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+    </row>
+    <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="64"/>
+      <c r="B5" s="62" t="n">
+        <v>200</v>
+      </c>
+      <c r="C5" s="62" t="n">
+        <v>76.83</v>
+      </c>
+      <c r="D5" s="62" t="n">
+        <v>77.47</v>
+      </c>
+      <c r="E5" s="62" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="F5" s="62" t="n">
+        <v>77.11</v>
+      </c>
+      <c r="G5" s="62" t="n">
+        <v>76.72</v>
+      </c>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+    </row>
+    <row r="6" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="64"/>
+      <c r="B6" s="62" t="n">
+        <v>600</v>
+      </c>
+      <c r="C6" s="62" t="n">
+        <v>76.94</v>
+      </c>
+      <c r="D6" s="62" t="n">
+        <v>76.63</v>
+      </c>
+      <c r="E6" s="62" t="n">
+        <v>76.91</v>
+      </c>
+      <c r="F6" s="62" t="n">
+        <v>76.68</v>
+      </c>
+      <c r="G6" s="62" t="n">
+        <v>76.88</v>
+      </c>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+    </row>
+    <row r="7" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="64"/>
+      <c r="B7" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="62" t="n">
+        <v>76.83</v>
+      </c>
+      <c r="D7" s="62" t="n">
+        <v>76.71</v>
+      </c>
+      <c r="E7" s="62" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="F7" s="62" t="n">
+        <v>76.99</v>
+      </c>
+      <c r="G7" s="62" t="n">
+        <v>77</v>
+      </c>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+    </row>
+    <row r="8" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="62"/>
+      <c r="B8" s="62" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C8" s="62" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+    </row>
+    <row r="9" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="62"/>
+      <c r="B9" s="62" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+    </row>
+    <row r="10" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="62"/>
+      <c r="B10" s="62" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+    </row>
+    <row r="11" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+    </row>
+    <row r="12" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="62"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+    </row>
+    <row r="13" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="60" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="63"/>
+    </row>
+    <row r="15" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="61" t="s">
+        <v>368</v>
+      </c>
+      <c r="B15" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="62" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" s="62" t="n">
+        <v>200</v>
+      </c>
+      <c r="F15" s="62" t="n">
+        <v>600</v>
+      </c>
+      <c r="G15" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H15" s="62" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I15" s="62" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J15" s="62" t="n">
+        <v>20000</v>
+      </c>
+      <c r="K15" s="63"/>
+      <c r="M15" s="63"/>
+    </row>
+    <row r="16" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="61"/>
+      <c r="B16" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62" t="n">
+        <v>78</v>
+      </c>
+      <c r="F16" s="62" t="n">
+        <v>75</v>
+      </c>
+      <c r="G16" s="62" t="n">
+        <v>75</v>
+      </c>
+      <c r="H16" s="62" t="n">
+        <v>73</v>
+      </c>
+      <c r="I16" s="62" t="n">
+        <v>74</v>
+      </c>
+      <c r="J16" s="62" t="n">
+        <v>74</v>
+      </c>
+      <c r="K16" s="63"/>
+    </row>
+    <row r="17" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="61"/>
+      <c r="B17" s="62" t="n">
+        <v>200</v>
+      </c>
+      <c r="C17" s="62" t="n">
+        <v>32</v>
+      </c>
+      <c r="D17" s="62" t="n">
+        <v>38</v>
+      </c>
+      <c r="E17" s="62" t="n">
+        <v>38.8</v>
+      </c>
+      <c r="F17" s="62" t="n">
+        <v>39</v>
+      </c>
+      <c r="G17" s="62" t="n">
+        <v>38</v>
+      </c>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="63"/>
+    </row>
+    <row r="18" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="61"/>
+      <c r="B18" s="62" t="n">
+        <v>600</v>
+      </c>
+      <c r="C18" s="62" t="n">
+        <v>34</v>
+      </c>
+      <c r="D18" s="62" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="E18" s="62" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="F18" s="62" t="n">
+        <v>33</v>
+      </c>
+      <c r="G18" s="62" t="n">
+        <v>33.2</v>
+      </c>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="63"/>
+    </row>
+    <row r="19" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="61"/>
+      <c r="B19" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="62" t="n">
+        <v>31</v>
+      </c>
+      <c r="D19" s="62" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="E19" s="62" t="n">
+        <v>31</v>
+      </c>
+      <c r="F19" s="62" t="n">
+        <v>31</v>
+      </c>
+      <c r="G19" s="62" t="n">
+        <v>31</v>
+      </c>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="63"/>
+    </row>
+    <row r="20" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="62"/>
+      <c r="B20" s="62" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C20" s="62" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="63"/>
+    </row>
+    <row r="21" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="62"/>
+      <c r="B21" s="62" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="63"/>
+    </row>
+    <row r="22" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="62"/>
+      <c r="B22" s="62" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="63"/>
+    </row>
+    <row r="23" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="62"/>
+      <c r="B23" s="62" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:A19"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Simulations in progress, files have been modified for testing, results updated in ErkParams.
</commit_message>
<xml_diff>
--- a/ErkParams.xlsx
+++ b/ErkParams.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="375">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -1887,19 +1887,37 @@
     <t xml:space="preserve">ppERK+MKP1&lt;-&gt; ppERKMKP1 &lt;-&gt; pERK+MKP1</t>
   </si>
   <si>
+    <t xml:space="preserve">Amplitude</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peakval</t>
   </si>
   <si>
     <t xml:space="preserve">CamCa4 (rate molecules/ms)</t>
   </si>
   <si>
-    <t xml:space="preserve">cAMP (rate molecules/ms)</t>
+    <t xml:space="preserve">cAMP/Gbg (rate molecules/ms)</t>
   </si>
   <si>
-    <t xml:space="preserve">T/2 s</t>
+    <t xml:space="preserve">T/2 </t>
   </si>
   <si>
-    <t xml:space="preserve">cAMP</t>
+    <t xml:space="preserve">cAMP/Gbg  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CamCa4 (duration/ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cAMP/Gbg (duration/s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cAMP/Gbg</t>
   </si>
 </sst>
 </file>
@@ -2187,7 +2205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2448,6 +2466,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2533,12 +2555,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="149.704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.4438775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="148.086734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3258,16 +3280,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.1530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4602,8 +4626,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="62" s="45" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0"/>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="47" t="s">
         <v>203</v>
       </c>
@@ -4732,7 +4755,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5295,10 +5318,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="54" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="54" width="110.15306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="54" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="54" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="54" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="54" width="108.938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="54" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56841,22 +56864,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.05"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="60" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="60" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="60" width="19.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="60" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="60" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="60" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61" t="s">
-        <v>364</v>
-      </c>
+      <c r="A1" s="61"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
       <c r="D1" s="62"/>
@@ -56872,7 +56895,7 @@
     </row>
     <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
@@ -56887,95 +56910,71 @@
       <c r="L2" s="63"/>
       <c r="M2" s="63"/>
     </row>
-    <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="64" t="s">
-        <v>366</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="62" t="n">
-        <v>100</v>
-      </c>
-      <c r="E3" s="62" t="n">
-        <v>200</v>
-      </c>
-      <c r="F3" s="62" t="n">
-        <v>600</v>
-      </c>
-      <c r="G3" s="62" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H3" s="62" t="n">
-        <v>1500</v>
-      </c>
-      <c r="I3" s="62" t="n">
-        <v>2000</v>
-      </c>
-      <c r="J3" s="62" t="n">
-        <v>20000</v>
-      </c>
+    <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="61" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
       <c r="K3" s="63"/>
       <c r="L3" s="63"/>
       <c r="M3" s="63"/>
     </row>
     <row r="4" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="64"/>
-      <c r="B4" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62" t="n">
-        <v>14.71</v>
-      </c>
-      <c r="F4" s="62" t="n">
-        <v>20.53</v>
-      </c>
-      <c r="G4" s="62" t="n">
-        <v>22.21</v>
-      </c>
-      <c r="H4" s="62" t="n">
-        <v>22.33</v>
-      </c>
-      <c r="I4" s="62" t="n">
-        <v>23.9</v>
-      </c>
-      <c r="J4" s="62" t="n">
-        <v>23.86</v>
-      </c>
+      <c r="A4" s="61" t="s">
+        <v>366</v>
+      </c>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
       <c r="K4" s="63"/>
       <c r="L4" s="63"/>
       <c r="M4" s="63"/>
     </row>
-    <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="64"/>
-      <c r="B5" s="62" t="n">
+    <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="64" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="62" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" s="62" t="n">
         <v>200</v>
       </c>
-      <c r="C5" s="62" t="n">
-        <v>76.83</v>
-      </c>
-      <c r="D5" s="62" t="n">
-        <v>77.47</v>
-      </c>
-      <c r="E5" s="62" t="n">
-        <v>77.5</v>
-      </c>
       <c r="F5" s="62" t="n">
-        <v>77.11</v>
+        <v>600</v>
       </c>
       <c r="G5" s="62" t="n">
-        <v>76.72</v>
-      </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
+        <v>1000</v>
+      </c>
+      <c r="H5" s="62" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I5" s="62" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J5" s="62" t="n">
+        <v>20000</v>
+      </c>
       <c r="K5" s="63"/>
       <c r="L5" s="63"/>
       <c r="M5" s="63"/>
@@ -56983,26 +56982,32 @@
     <row r="6" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="64"/>
       <c r="B6" s="62" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="C6" s="62" t="n">
-        <v>76.94</v>
+        <v>0</v>
       </c>
       <c r="D6" s="62" t="n">
-        <v>76.63</v>
+        <v>7.27</v>
       </c>
       <c r="E6" s="62" t="n">
-        <v>76.91</v>
+        <v>14.71</v>
       </c>
       <c r="F6" s="62" t="n">
-        <v>76.68</v>
+        <v>20.53</v>
       </c>
       <c r="G6" s="62" t="n">
-        <v>76.88</v>
-      </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
+        <v>22.21</v>
+      </c>
+      <c r="H6" s="62" t="n">
+        <v>22.33</v>
+      </c>
+      <c r="I6" s="62" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="J6" s="62" t="n">
+        <v>23.86</v>
+      </c>
       <c r="K6" s="63"/>
       <c r="L6" s="63"/>
       <c r="M6" s="63"/>
@@ -57010,62 +57015,98 @@
     <row r="7" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="64"/>
       <c r="B7" s="62" t="n">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="C7" s="62" t="n">
         <v>76.83</v>
       </c>
       <c r="D7" s="62" t="n">
-        <v>76.71</v>
+        <v>77.47</v>
       </c>
       <c r="E7" s="62" t="n">
-        <v>76.5</v>
+        <v>77.5</v>
       </c>
       <c r="F7" s="62" t="n">
-        <v>76.99</v>
+        <v>77.11</v>
       </c>
       <c r="G7" s="62" t="n">
-        <v>77</v>
-      </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
+        <v>76.72</v>
+      </c>
+      <c r="H7" s="62" t="n">
+        <v>77.47</v>
+      </c>
+      <c r="I7" s="62" t="n">
+        <v>77.3</v>
+      </c>
+      <c r="J7" s="62" t="n">
+        <v>77.49</v>
+      </c>
       <c r="K7" s="63"/>
       <c r="L7" s="63"/>
       <c r="M7" s="63"/>
     </row>
     <row r="8" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="62"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="62" t="n">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="C8" s="62" t="n">
-        <v>77.2</v>
-      </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
+        <v>76.94</v>
+      </c>
+      <c r="D8" s="62" t="n">
+        <v>76.63</v>
+      </c>
+      <c r="E8" s="62" t="n">
+        <v>76.91</v>
+      </c>
+      <c r="F8" s="62" t="n">
+        <v>76.68</v>
+      </c>
+      <c r="G8" s="62" t="n">
+        <v>76.88</v>
+      </c>
+      <c r="H8" s="62" t="n">
+        <v>76.26</v>
+      </c>
+      <c r="I8" s="62" t="n">
+        <v>76.91</v>
+      </c>
+      <c r="J8" s="62" t="n">
+        <v>77.22</v>
+      </c>
       <c r="K8" s="63"/>
       <c r="L8" s="63"/>
       <c r="M8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="62"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="62" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
+        <v>1000</v>
+      </c>
+      <c r="C9" s="62" t="n">
+        <v>76.83</v>
+      </c>
+      <c r="D9" s="62" t="n">
+        <v>76.71</v>
+      </c>
+      <c r="E9" s="62" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="F9" s="62" t="n">
+        <v>76.99</v>
+      </c>
+      <c r="G9" s="62" t="n">
+        <v>77</v>
+      </c>
+      <c r="H9" s="62" t="n">
+        <v>76.74</v>
+      </c>
+      <c r="I9" s="62" t="n">
+        <v>77.22</v>
+      </c>
+      <c r="J9" s="62" t="n">
+        <v>76.94</v>
+      </c>
       <c r="K9" s="63"/>
       <c r="L9" s="63"/>
       <c r="M9" s="63"/>
@@ -57073,54 +57114,117 @@
     <row r="10" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="62"/>
       <c r="B10" s="62" t="n">
-        <v>20000</v>
-      </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
+        <v>1500</v>
+      </c>
+      <c r="C10" s="62" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="D10" s="62" t="n">
+        <v>76.49</v>
+      </c>
+      <c r="E10" s="62" t="n">
+        <v>76.64</v>
+      </c>
+      <c r="F10" s="62" t="n">
+        <v>76.69</v>
+      </c>
+      <c r="G10" s="62" t="n">
+        <v>76.71</v>
+      </c>
+      <c r="H10" s="62" t="n">
+        <v>76.88</v>
+      </c>
+      <c r="I10" s="62" t="n">
+        <v>76.8</v>
+      </c>
+      <c r="J10" s="62" t="n">
+        <v>76.72</v>
+      </c>
       <c r="K10" s="63"/>
       <c r="L10" s="63"/>
       <c r="M10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="62"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
+      <c r="B11" s="62" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C11" s="62" t="n">
+        <v>76.52</v>
+      </c>
+      <c r="D11" s="62" t="n">
+        <v>76.56</v>
+      </c>
+      <c r="E11" s="62" t="n">
+        <v>76.57</v>
+      </c>
+      <c r="F11" s="62" t="n">
+        <v>76.76</v>
+      </c>
+      <c r="G11" s="62" t="n">
+        <v>77.11</v>
+      </c>
+      <c r="H11" s="62" t="n">
+        <v>76.89</v>
+      </c>
+      <c r="I11" s="62" t="n">
+        <v>76.95</v>
+      </c>
+      <c r="J11" s="62" t="n">
+        <v>77.41</v>
+      </c>
       <c r="K11" s="63"/>
       <c r="L11" s="63"/>
       <c r="M11" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
+      <c r="B12" s="62" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C12" s="62" t="n">
+        <v>76.44</v>
+      </c>
+      <c r="D12" s="62" t="n">
+        <v>77.05</v>
+      </c>
+      <c r="E12" s="62" t="n">
+        <v>76.43</v>
+      </c>
+      <c r="F12" s="62" t="n">
+        <v>76.57</v>
+      </c>
+      <c r="G12" s="62" t="n">
+        <v>76.73</v>
+      </c>
+      <c r="H12" s="62" t="n">
+        <v>76.82</v>
+      </c>
+      <c r="I12" s="62" t="n">
+        <v>76.72</v>
+      </c>
+      <c r="J12" s="62" t="n">
+        <v>76.44</v>
+      </c>
       <c r="K12" s="63"/>
       <c r="L12" s="63"/>
       <c r="M12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="60" t="s">
-        <v>367</v>
-      </c>
+        <v>368</v>
+      </c>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="M13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="61" t="s">
@@ -57136,10 +57240,11 @@
       <c r="I14" s="62"/>
       <c r="J14" s="62"/>
       <c r="K14" s="63"/>
+      <c r="M14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="61" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B15" s="62" t="s">
         <v>47</v>
@@ -57179,24 +57284,26 @@
       <c r="C16" s="62" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="62"/>
+      <c r="D16" s="62" t="n">
+        <v>0.7</v>
+      </c>
       <c r="E16" s="62" t="n">
-        <v>78</v>
+        <v>1.7</v>
       </c>
       <c r="F16" s="62" t="n">
-        <v>75</v>
+        <v>2.4</v>
       </c>
       <c r="G16" s="62" t="n">
-        <v>75</v>
+        <v>3.3</v>
       </c>
       <c r="H16" s="62" t="n">
-        <v>73</v>
+        <v>3.32</v>
       </c>
       <c r="I16" s="62" t="n">
-        <v>74</v>
+        <v>3.1</v>
       </c>
       <c r="J16" s="62" t="n">
-        <v>74</v>
+        <v>2.7</v>
       </c>
       <c r="K16" s="63"/>
     </row>
@@ -57220,9 +57327,15 @@
       <c r="G17" s="62" t="n">
         <v>38</v>
       </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
+      <c r="H17" s="62" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="I17" s="62" t="n">
+        <v>44</v>
+      </c>
+      <c r="J17" s="62" t="n">
+        <v>38.4</v>
+      </c>
       <c r="K17" s="63"/>
     </row>
     <row r="18" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57243,11 +57356,17 @@
         <v>33</v>
       </c>
       <c r="G18" s="62" t="n">
-        <v>33.2</v>
-      </c>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
+        <v>38.4</v>
+      </c>
+      <c r="H18" s="62" t="n">
+        <v>37</v>
+      </c>
+      <c r="I18" s="62" t="n">
+        <v>39</v>
+      </c>
+      <c r="J18" s="62" t="n">
+        <v>49.8</v>
+      </c>
       <c r="K18" s="63"/>
     </row>
     <row r="19" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57270,9 +57389,15 @@
       <c r="G19" s="62" t="n">
         <v>31</v>
       </c>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
+      <c r="H19" s="62" t="n">
+        <v>41</v>
+      </c>
+      <c r="I19" s="62" t="n">
+        <v>49.1</v>
+      </c>
+      <c r="J19" s="62" t="n">
+        <v>64</v>
+      </c>
       <c r="K19" s="63"/>
     </row>
     <row r="20" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57283,13 +57408,27 @@
       <c r="C20" s="62" t="n">
         <v>30.5</v>
       </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
+      <c r="D20" s="62" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="E20" s="62" t="n">
+        <v>33.2</v>
+      </c>
+      <c r="F20" s="62" t="n">
+        <v>53</v>
+      </c>
+      <c r="G20" s="62" t="n">
+        <v>51</v>
+      </c>
+      <c r="H20" s="62" t="n">
+        <v>52</v>
+      </c>
+      <c r="I20" s="62" t="n">
+        <v>49.6</v>
+      </c>
+      <c r="J20" s="62" t="n">
+        <v>43.3</v>
+      </c>
       <c r="K20" s="63"/>
     </row>
     <row r="21" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57297,52 +57436,436 @@
       <c r="B21" s="62" t="n">
         <v>2000</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
+      <c r="C21" s="62" t="n">
+        <v>32</v>
+      </c>
+      <c r="D21" s="62" t="n">
+        <v>42.4</v>
+      </c>
+      <c r="E21" s="62" t="n">
+        <v>52</v>
+      </c>
+      <c r="F21" s="62" t="n">
+        <v>43.2</v>
+      </c>
+      <c r="G21" s="62" t="n">
+        <v>39</v>
+      </c>
+      <c r="H21" s="62" t="n">
+        <v>42</v>
+      </c>
+      <c r="I21" s="62" t="n">
+        <v>45</v>
+      </c>
+      <c r="J21" s="62" t="n">
+        <v>47</v>
+      </c>
       <c r="K21" s="63"/>
     </row>
     <row r="22" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="62"/>
       <c r="B22" s="62" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
+        <v>20000</v>
+      </c>
+      <c r="C22" s="62" t="n">
+        <v>49</v>
+      </c>
+      <c r="D22" s="62" t="n">
+        <v>52</v>
+      </c>
+      <c r="E22" s="62" t="n">
+        <v>33.6</v>
+      </c>
+      <c r="F22" s="62" t="n">
+        <v>44.6</v>
+      </c>
+      <c r="G22" s="62" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="H22" s="62" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="I22" s="62" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="J22" s="62" t="n">
+        <v>35.5</v>
+      </c>
       <c r="K22" s="63"/>
     </row>
-    <row r="23" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="62"/>
-      <c r="B23" s="62" t="n">
-        <v>3000</v>
-      </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="63"/>
+    <row r="23" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="61" t="s">
+        <v>370</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+    </row>
+    <row r="26" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="61" t="s">
+        <v>365</v>
+      </c>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+    </row>
+    <row r="27" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="61" t="s">
+        <v>371</v>
+      </c>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+    </row>
+    <row r="28" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="64" t="s">
+        <v>372</v>
+      </c>
+      <c r="B28" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="62" t="n">
+        <v>100</v>
+      </c>
+      <c r="E28" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F28" s="62" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G28" s="62" t="n">
+        <v>100000</v>
+      </c>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+    </row>
+    <row r="29" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="64"/>
+      <c r="B29" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="62" t="n">
+        <v>13.81</v>
+      </c>
+      <c r="E29" s="62" t="n">
+        <v>22.32</v>
+      </c>
+      <c r="F29" s="62" t="n">
+        <v>23.35</v>
+      </c>
+      <c r="G29" s="62" t="n">
+        <v>23.85</v>
+      </c>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+    </row>
+    <row r="30" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="64"/>
+      <c r="B30" s="62" t="n">
+        <v>100</v>
+      </c>
+      <c r="C30" s="62" t="n">
+        <v>77.22</v>
+      </c>
+      <c r="D30" s="62" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="E30" s="62" t="n">
+        <v>76.67</v>
+      </c>
+      <c r="F30" s="62" t="n">
+        <v>76.55</v>
+      </c>
+      <c r="G30" s="62" t="n">
+        <v>76.9</v>
+      </c>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+    </row>
+    <row r="31" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="64"/>
+      <c r="B31" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C31" s="62" t="n">
+        <v>76.39</v>
+      </c>
+      <c r="D31" s="62" t="n">
+        <v>76.52</v>
+      </c>
+      <c r="E31" s="62" t="n">
+        <v>77.39</v>
+      </c>
+      <c r="F31" s="62" t="n">
+        <v>77.15</v>
+      </c>
+      <c r="G31" s="62" t="n">
+        <v>77.02</v>
+      </c>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+    </row>
+    <row r="32" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="64"/>
+      <c r="B32" s="62" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C32" s="62" t="n">
+        <v>77.24</v>
+      </c>
+      <c r="D32" s="62" t="n">
+        <v>77.08</v>
+      </c>
+      <c r="E32" s="62" t="n">
+        <v>76.87</v>
+      </c>
+      <c r="F32" s="62" t="n">
+        <v>77.4</v>
+      </c>
+      <c r="G32" s="62" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+    </row>
+    <row r="33" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="62"/>
+      <c r="B33" s="62" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C33" s="62" t="n">
+        <v>76.72</v>
+      </c>
+      <c r="D33" s="62" t="n">
+        <v>76.83</v>
+      </c>
+      <c r="E33" s="62" t="n">
+        <v>77.03</v>
+      </c>
+      <c r="F33" s="62" t="n">
+        <v>76.84</v>
+      </c>
+      <c r="G33" s="62" t="n">
+        <v>76.65</v>
+      </c>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+    </row>
+    <row r="34" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="60" t="s">
+        <v>373</v>
+      </c>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+    </row>
+    <row r="36" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="61" t="s">
+        <v>374</v>
+      </c>
+      <c r="B36" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="62" t="n">
+        <v>100</v>
+      </c>
+      <c r="E36" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F36" s="62" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G36" s="62" t="n">
+        <v>100000</v>
+      </c>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
+    </row>
+    <row r="37" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="61"/>
+      <c r="B37" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="62" t="n">
+        <v>10</v>
+      </c>
+      <c r="D37" s="62" t="n">
+        <v>99.94</v>
+      </c>
+      <c r="E37" s="62" t="n">
+        <v>99.98</v>
+      </c>
+      <c r="F37" s="62" t="n">
+        <v>99.5</v>
+      </c>
+      <c r="G37" s="62" t="n">
+        <v>99.96</v>
+      </c>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+    </row>
+    <row r="38" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="61"/>
+      <c r="B38" s="62" t="n">
+        <v>100</v>
+      </c>
+      <c r="C38" s="62" t="n">
+        <v>74.82</v>
+      </c>
+      <c r="D38" s="62" t="n">
+        <v>81.66</v>
+      </c>
+      <c r="E38" s="62" t="n">
+        <v>89.72</v>
+      </c>
+      <c r="F38" s="62" t="n">
+        <v>81.66</v>
+      </c>
+      <c r="G38" s="62" t="n">
+        <v>74.64</v>
+      </c>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
+    </row>
+    <row r="39" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="61"/>
+      <c r="B39" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C39" s="62" t="n">
+        <v>61.74</v>
+      </c>
+      <c r="D39" s="62" t="n">
+        <v>66.8</v>
+      </c>
+      <c r="E39" s="62" t="n">
+        <v>68.64</v>
+      </c>
+      <c r="F39" s="62" t="n">
+        <v>63.7</v>
+      </c>
+      <c r="G39" s="62" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+    </row>
+    <row r="40" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="61"/>
+      <c r="B40" s="62" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C40" s="62" t="n">
+        <v>73.08</v>
+      </c>
+      <c r="D40" s="62" t="n">
+        <v>68.3</v>
+      </c>
+      <c r="E40" s="62" t="n">
+        <v>62.78</v>
+      </c>
+      <c r="F40" s="62" t="n">
+        <v>76.32</v>
+      </c>
+      <c r="G40" s="62" t="n">
+        <v>64.06</v>
+      </c>
+      <c r="H40" s="63"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="63"/>
+    </row>
+    <row r="41" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="62"/>
+      <c r="B41" s="62" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C41" s="62" t="n">
+        <v>69.48</v>
+      </c>
+      <c r="D41" s="62" t="n">
+        <v>60.92</v>
+      </c>
+      <c r="E41" s="62" t="n">
+        <v>77.14</v>
+      </c>
+      <c r="F41" s="62" t="n">
+        <v>61.08</v>
+      </c>
+      <c r="G41" s="62" t="n">
+        <v>70.66</v>
+      </c>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="10">
     <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:A9"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:A40"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>